<commit_message>
Updates the spectral reflectance plot (supplement)
</commit_message>
<xml_diff>
--- a/tables/Manuscript_Tables.xlsx
+++ b/tables/Manuscript_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6270a8f4b8f62cae/mcook/earth-lab/opp-rooftop-mapping/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1447" documentId="8_{8DE99770-8E62-3C41-974E-AE408B9D5CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD01F082-2C11-AF4E-BC34-D843C708C0FF}"/>
+  <xr:revisionPtr revIDLastSave="1448" documentId="8_{8DE99770-8E62-3C41-974E-AE408B9D5CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB0E4C88-C07D-8748-848D-47AFFADA4235}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="20" yWindow="760" windowWidth="30240" windowHeight="17880" activeTab="4" xr2:uid="{CB73D5E9-BD95-EA4F-8517-9430AC64DA52}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" activeTab="6" xr2:uid="{CB73D5E9-BD95-EA4F-8517-9430AC64DA52}"/>
   </bookViews>
   <sheets>
     <sheet name="Class Descriptions" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Table 2.Accuracy" sheetId="1" r:id="rId4"/>
     <sheet name="S.Table1.AreaDistance Clean" sheetId="6" r:id="rId5"/>
     <sheet name="S.Table1.AreaDistance" sheetId="4" r:id="rId6"/>
+    <sheet name="Classification report (DC)" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="120">
   <si>
     <t>Material</t>
   </si>
@@ -386,16 +387,32 @@
   </si>
   <si>
     <t>Mean Area (m2)</t>
+  </si>
+  <si>
+    <t>Weighted average</t>
+  </si>
+  <si>
+    <t>Wood shingle</t>
+  </si>
+  <si>
+    <t>Tar &amp; gravel</t>
+  </si>
+  <si>
+    <t>Denver, CO</t>
+  </si>
+  <si>
+    <t>Washington, D.C.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -496,6 +513,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -511,7 +536,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -772,11 +797,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -931,6 +967,156 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -949,178 +1135,43 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1875,7 +1926,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:N26"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1883,7 +1934,7 @@
     <col min="1" max="1" width="6.6640625" style="24" customWidth="1"/>
     <col min="2" max="2" width="6.1640625" style="24" customWidth="1"/>
     <col min="3" max="3" width="8" style="24" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="68" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="24" customWidth="1"/>
     <col min="5" max="5" width="3.33203125" style="26" customWidth="1"/>
     <col min="6" max="9" width="7.33203125" style="24" customWidth="1"/>
     <col min="10" max="10" width="4.83203125" style="24" customWidth="1"/>
@@ -1895,7 +1946,7 @@
       <c r="A1" s="27"/>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
-      <c r="D1" s="66"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="28"/>
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
@@ -1910,878 +1961,878 @@
     </row>
     <row r="2" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="71" t="s">
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="75" t="s">
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="76"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="104"/>
       <c r="O2" s="27"/>
     </row>
     <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="27"/>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="78"/>
-      <c r="F3" s="77" t="s">
+      <c r="E3" s="62"/>
+      <c r="F3" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="77" t="s">
+      <c r="G3" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="77" t="s">
+      <c r="I3" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="79"/>
-      <c r="K3" s="77" t="s">
+      <c r="J3" s="63"/>
+      <c r="K3" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="77" t="s">
+      <c r="L3" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="77" t="s">
+      <c r="M3" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="77" t="s">
+      <c r="N3" s="61" t="s">
         <v>11</v>
       </c>
       <c r="O3" s="27"/>
     </row>
     <row r="4" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="27"/>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="82"/>
-      <c r="F4" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="G4" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="J4" s="83"/>
-      <c r="K4" s="84">
+      <c r="E4" s="65"/>
+      <c r="F4" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" s="66"/>
+      <c r="K4" s="67">
         <v>0.77407800000000004</v>
       </c>
-      <c r="L4" s="85">
+      <c r="L4" s="68">
         <v>0.930419</v>
       </c>
-      <c r="M4" s="85">
+      <c r="M4" s="68">
         <v>0.845078</v>
       </c>
-      <c r="N4" s="86">
+      <c r="N4" s="69">
         <v>1624</v>
       </c>
       <c r="O4" s="27"/>
     </row>
     <row r="5" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27"/>
-      <c r="B5" s="87"/>
-      <c r="C5" s="81" t="s">
+      <c r="B5" s="98"/>
+      <c r="C5" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="81" t="s">
+      <c r="D5" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="82"/>
-      <c r="F5" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="G5" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="H5" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="I5" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84">
+      <c r="E5" s="65"/>
+      <c r="F5" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" s="66"/>
+      <c r="K5" s="67">
         <v>0.70294100000000004</v>
       </c>
-      <c r="L5" s="84">
+      <c r="L5" s="67">
         <v>0.86594199999999999</v>
       </c>
-      <c r="M5" s="84">
+      <c r="M5" s="67">
         <v>0.77597400000000005</v>
       </c>
-      <c r="N5" s="86">
+      <c r="N5" s="69">
         <v>552</v>
       </c>
       <c r="O5" s="27"/>
     </row>
     <row r="6" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
-      <c r="B6" s="87"/>
-      <c r="C6" s="81" t="s">
+      <c r="B6" s="98"/>
+      <c r="C6" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="81" t="s">
+      <c r="D6" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="88">
+      <c r="E6" s="65"/>
+      <c r="F6" s="70">
         <v>0.79821399999999998</v>
       </c>
-      <c r="G6" s="88">
+      <c r="G6" s="70">
         <v>0.62582499999999996</v>
       </c>
-      <c r="H6" s="88">
+      <c r="H6" s="70">
         <v>0.70158500000000001</v>
       </c>
-      <c r="I6" s="81">
+      <c r="I6" s="64">
         <v>7427</v>
       </c>
-      <c r="J6" s="83"/>
-      <c r="K6" s="84">
+      <c r="J6" s="66"/>
+      <c r="K6" s="67">
         <v>0.96874400000000005</v>
       </c>
-      <c r="L6" s="84">
+      <c r="L6" s="67">
         <v>0.92554700000000001</v>
       </c>
-      <c r="M6" s="84">
+      <c r="M6" s="67">
         <v>0.94665299999999997</v>
       </c>
-      <c r="N6" s="86">
+      <c r="N6" s="69">
         <v>17313</v>
       </c>
       <c r="O6" s="27"/>
     </row>
     <row r="7" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="81" t="s">
+      <c r="B7" s="98"/>
+      <c r="C7" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="81" t="s">
+      <c r="D7" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="82"/>
-      <c r="F7" s="85">
+      <c r="E7" s="65"/>
+      <c r="F7" s="68">
         <v>0.87615600000000005</v>
       </c>
-      <c r="G7" s="85">
+      <c r="G7" s="68">
         <v>0.74555800000000005</v>
       </c>
-      <c r="H7" s="85">
+      <c r="H7" s="68">
         <v>0.80559800000000004</v>
       </c>
-      <c r="I7" s="86">
+      <c r="I7" s="69">
         <v>7373</v>
       </c>
-      <c r="J7" s="83"/>
-      <c r="K7" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="L7" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="M7" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="N7" s="81" t="s">
+      <c r="J7" s="66"/>
+      <c r="K7" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" s="64" t="s">
         <v>80</v>
       </c>
       <c r="O7" s="27"/>
     </row>
     <row r="8" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
-      <c r="B8" s="87"/>
-      <c r="C8" s="81" t="s">
+      <c r="B8" s="98"/>
+      <c r="C8" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="81" t="s">
+      <c r="D8" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="82"/>
-      <c r="F8" s="89">
+      <c r="E8" s="65"/>
+      <c r="F8" s="71">
         <v>0.109333</v>
       </c>
-      <c r="G8" s="89">
+      <c r="G8" s="71">
         <v>0.26114599999999999</v>
       </c>
-      <c r="H8" s="89">
+      <c r="H8" s="71">
         <v>0.15413499999999999</v>
       </c>
-      <c r="I8" s="90">
+      <c r="I8" s="72">
         <v>157</v>
       </c>
-      <c r="J8" s="83"/>
-      <c r="K8" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="L8" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="M8" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="N8" s="81" t="s">
+      <c r="J8" s="66"/>
+      <c r="K8" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="M8" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="N8" s="64" t="s">
         <v>80</v>
       </c>
       <c r="O8" s="27"/>
     </row>
     <row r="9" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="87"/>
-      <c r="C9" s="81" t="s">
+      <c r="B9" s="98"/>
+      <c r="C9" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="81" t="s">
+      <c r="D9" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="82"/>
-      <c r="F9" s="85">
+      <c r="E9" s="65"/>
+      <c r="F9" s="68">
         <v>0.478271</v>
       </c>
-      <c r="G9" s="85">
+      <c r="G9" s="68">
         <v>0.670269</v>
       </c>
-      <c r="H9" s="85">
+      <c r="H9" s="68">
         <v>0.558222</v>
       </c>
-      <c r="I9" s="86">
+      <c r="I9" s="69">
         <v>3054</v>
       </c>
-      <c r="J9" s="83"/>
-      <c r="K9" s="88">
+      <c r="J9" s="66"/>
+      <c r="K9" s="70">
         <v>0</v>
       </c>
-      <c r="L9" s="88">
+      <c r="L9" s="70">
         <v>0</v>
       </c>
-      <c r="M9" s="88">
+      <c r="M9" s="70">
         <v>0</v>
       </c>
-      <c r="N9" s="81">
+      <c r="N9" s="64">
         <v>46</v>
       </c>
       <c r="O9" s="27"/>
     </row>
     <row r="10" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
-      <c r="B10" s="87"/>
-      <c r="C10" s="81" t="s">
+      <c r="B10" s="98"/>
+      <c r="C10" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="81" t="s">
+      <c r="D10" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="82"/>
-      <c r="F10" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="83"/>
-      <c r="K10" s="84">
+      <c r="E10" s="65"/>
+      <c r="F10" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="66"/>
+      <c r="K10" s="67">
         <v>0.12837799999999999</v>
       </c>
-      <c r="L10" s="84">
+      <c r="L10" s="67">
         <v>0.41304299999999999</v>
       </c>
-      <c r="M10" s="84">
+      <c r="M10" s="67">
         <v>0.19587599999999999</v>
       </c>
-      <c r="N10" s="86">
+      <c r="N10" s="69">
         <v>46</v>
       </c>
       <c r="O10" s="27"/>
     </row>
     <row r="11" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
-      <c r="B11" s="87"/>
-      <c r="C11" s="81" t="s">
+      <c r="B11" s="98"/>
+      <c r="C11" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="81" t="s">
+      <c r="D11" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="82"/>
-      <c r="F11" s="88">
+      <c r="E11" s="65"/>
+      <c r="F11" s="70">
         <v>0.242647</v>
       </c>
-      <c r="G11" s="88">
+      <c r="G11" s="70">
         <v>0.35675699999999999</v>
       </c>
-      <c r="H11" s="88">
+      <c r="H11" s="70">
         <v>0.28883999999999999</v>
       </c>
-      <c r="I11" s="81">
+      <c r="I11" s="64">
         <v>185</v>
       </c>
-      <c r="J11" s="83"/>
-      <c r="K11" s="85">
+      <c r="J11" s="66"/>
+      <c r="K11" s="68">
         <v>0.59212399999999998</v>
       </c>
-      <c r="L11" s="85">
+      <c r="L11" s="68">
         <v>0.73989499999999997</v>
       </c>
-      <c r="M11" s="85">
+      <c r="M11" s="68">
         <v>0.65781299999999998</v>
       </c>
-      <c r="N11" s="86">
+      <c r="N11" s="69">
         <v>569</v>
       </c>
       <c r="O11" s="27"/>
     </row>
     <row r="12" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
-      <c r="B12" s="87"/>
-      <c r="C12" s="81" t="s">
+      <c r="B12" s="98"/>
+      <c r="C12" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="81" t="s">
+      <c r="D12" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="82"/>
-      <c r="F12" s="85">
+      <c r="E12" s="65"/>
+      <c r="F12" s="68">
         <v>0.144455</v>
       </c>
-      <c r="G12" s="85">
+      <c r="G12" s="68">
         <v>0.60546900000000003</v>
       </c>
-      <c r="H12" s="85">
+      <c r="H12" s="68">
         <v>0.23325799999999999</v>
       </c>
-      <c r="I12" s="86">
+      <c r="I12" s="69">
         <v>256</v>
       </c>
-      <c r="J12" s="83"/>
-      <c r="K12" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="L12" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="M12" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="N12" s="81" t="s">
+      <c r="J12" s="66"/>
+      <c r="K12" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="L12" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="M12" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="N12" s="64" t="s">
         <v>80</v>
       </c>
       <c r="O12" s="27"/>
     </row>
     <row r="13" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
-      <c r="B13" s="87"/>
-      <c r="C13" s="91" t="s">
+      <c r="B13" s="98"/>
+      <c r="C13" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="91" t="s">
+      <c r="D13" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="92"/>
-      <c r="F13" s="93">
+      <c r="E13" s="74"/>
+      <c r="F13" s="75">
         <v>0.14505100000000001</v>
       </c>
-      <c r="G13" s="93">
+      <c r="G13" s="75">
         <v>0.36796499999999999</v>
       </c>
-      <c r="H13" s="93">
+      <c r="H13" s="75">
         <v>0.20807800000000001</v>
       </c>
-      <c r="I13" s="91">
+      <c r="I13" s="73">
         <v>231</v>
       </c>
-      <c r="J13" s="94"/>
-      <c r="K13" s="95">
+      <c r="J13" s="76"/>
+      <c r="K13" s="77">
         <v>0.61904800000000004</v>
       </c>
-      <c r="L13" s="95">
+      <c r="L13" s="77">
         <v>0.65335799999999999</v>
       </c>
-      <c r="M13" s="95">
+      <c r="M13" s="77">
         <v>0.63573999999999997</v>
       </c>
-      <c r="N13" s="96">
+      <c r="N13" s="78">
         <v>2129</v>
       </c>
       <c r="O13" s="27"/>
     </row>
     <row r="14" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
-      <c r="B14" s="97"/>
-      <c r="C14" s="98" t="s">
+      <c r="B14" s="79"/>
+      <c r="C14" s="96" t="s">
         <v>93</v>
       </c>
-      <c r="D14" s="98"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="99">
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="106">
         <v>0.69799999999999995</v>
       </c>
-      <c r="G14" s="99"/>
-      <c r="H14" s="99"/>
-      <c r="I14" s="99"/>
-      <c r="J14" s="100"/>
-      <c r="K14" s="99">
+      <c r="G14" s="106"/>
+      <c r="H14" s="106"/>
+      <c r="I14" s="106"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="106">
         <v>0.89439999999999997</v>
       </c>
-      <c r="L14" s="99"/>
-      <c r="M14" s="99"/>
-      <c r="N14" s="99"/>
+      <c r="L14" s="106"/>
+      <c r="M14" s="106"/>
+      <c r="N14" s="106"/>
       <c r="O14" s="27"/>
     </row>
     <row r="15" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="102" t="s">
+      <c r="C15" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="102" t="s">
+      <c r="D15" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="103"/>
-      <c r="F15" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="I15" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" s="104"/>
-      <c r="K15" s="105">
+      <c r="E15" s="65"/>
+      <c r="F15" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" s="81"/>
+      <c r="K15" s="82">
         <v>0.79813699999999999</v>
       </c>
-      <c r="L15" s="105">
+      <c r="L15" s="82">
         <v>0.47475400000000001</v>
       </c>
-      <c r="M15" s="105">
+      <c r="M15" s="82">
         <v>0.59536699999999998</v>
       </c>
-      <c r="N15" s="102">
+      <c r="N15" s="64">
         <v>1624</v>
       </c>
       <c r="O15" s="27"/>
     </row>
     <row r="16" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
-      <c r="B16" s="101"/>
-      <c r="C16" s="102" t="s">
+      <c r="B16" s="98"/>
+      <c r="C16" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="102" t="s">
+      <c r="D16" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="103"/>
-      <c r="F16" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="G16" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="I16" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="J16" s="83"/>
-      <c r="K16" s="105">
+      <c r="E16" s="65"/>
+      <c r="F16" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="66"/>
+      <c r="K16" s="82">
         <v>0.303207</v>
       </c>
-      <c r="L16" s="105">
+      <c r="L16" s="82">
         <v>0.18840599999999999</v>
       </c>
-      <c r="M16" s="105">
+      <c r="M16" s="82">
         <v>0.232402</v>
       </c>
-      <c r="N16" s="102">
+      <c r="N16" s="64">
         <v>552</v>
       </c>
       <c r="O16" s="27"/>
     </row>
     <row r="17" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27"/>
-      <c r="B17" s="101"/>
-      <c r="C17" s="102" t="s">
+      <c r="B17" s="98"/>
+      <c r="C17" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="102" t="s">
+      <c r="D17" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="103"/>
-      <c r="F17" s="106">
+      <c r="E17" s="65"/>
+      <c r="F17" s="70">
         <v>0.71347700000000003</v>
       </c>
-      <c r="G17" s="106">
+      <c r="G17" s="70">
         <v>0.52605400000000002</v>
       </c>
-      <c r="H17" s="106">
+      <c r="H17" s="70">
         <v>0.60559600000000002</v>
       </c>
-      <c r="I17" s="102">
+      <c r="I17" s="64">
         <v>7427</v>
       </c>
-      <c r="J17" s="83"/>
-      <c r="K17" s="105">
+      <c r="J17" s="66"/>
+      <c r="K17" s="82">
         <v>0.82968299999999995</v>
       </c>
-      <c r="L17" s="105">
+      <c r="L17" s="82">
         <v>0.94963299999999995</v>
       </c>
-      <c r="M17" s="105">
+      <c r="M17" s="82">
         <v>0.88561500000000004</v>
       </c>
-      <c r="N17" s="102">
+      <c r="N17" s="64">
         <v>17313</v>
       </c>
       <c r="O17" s="27"/>
     </row>
     <row r="18" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
-      <c r="B18" s="101"/>
-      <c r="C18" s="102" t="s">
+      <c r="B18" s="98"/>
+      <c r="C18" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="102" t="s">
+      <c r="D18" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="103"/>
-      <c r="F18" s="106">
+      <c r="E18" s="65"/>
+      <c r="F18" s="70">
         <v>0.79953700000000005</v>
       </c>
-      <c r="G18" s="106">
+      <c r="G18" s="70">
         <v>0.70215700000000003</v>
       </c>
-      <c r="H18" s="105">
+      <c r="H18" s="82">
         <v>0.74768900000000005</v>
       </c>
-      <c r="I18" s="102">
+      <c r="I18" s="64">
         <v>7373</v>
       </c>
-      <c r="J18" s="83"/>
-      <c r="K18" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="L18" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="M18" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="N18" s="102" t="s">
+      <c r="J18" s="66"/>
+      <c r="K18" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="L18" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="M18" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="N18" s="64" t="s">
         <v>80</v>
       </c>
       <c r="O18" s="27"/>
     </row>
     <row r="19" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
-      <c r="B19" s="101"/>
-      <c r="C19" s="102" t="s">
+      <c r="B19" s="98"/>
+      <c r="C19" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="102" t="s">
+      <c r="D19" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="103"/>
-      <c r="F19" s="106">
+      <c r="E19" s="65"/>
+      <c r="F19" s="70">
         <v>3.5714000000000003E-2</v>
       </c>
-      <c r="G19" s="105">
+      <c r="G19" s="82">
         <v>2.5478000000000001E-2</v>
       </c>
-      <c r="H19" s="105">
+      <c r="H19" s="82">
         <v>2.9739999999999999E-2</v>
       </c>
-      <c r="I19" s="102">
+      <c r="I19" s="64">
         <v>157</v>
       </c>
-      <c r="J19" s="83"/>
-      <c r="K19" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="L19" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="M19" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="N19" s="102" t="s">
+      <c r="J19" s="66"/>
+      <c r="K19" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="L19" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="M19" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="N19" s="64" t="s">
         <v>80</v>
       </c>
       <c r="O19" s="27"/>
     </row>
     <row r="20" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
-      <c r="B20" s="101"/>
-      <c r="C20" s="102" t="s">
+      <c r="B20" s="98"/>
+      <c r="C20" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="102" t="s">
+      <c r="D20" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="103"/>
-      <c r="F20" s="106">
+      <c r="E20" s="65"/>
+      <c r="F20" s="70">
         <v>0.37269099999999999</v>
       </c>
-      <c r="G20" s="106">
+      <c r="G20" s="70">
         <v>0.55501</v>
       </c>
-      <c r="H20" s="106">
+      <c r="H20" s="70">
         <v>0.44593500000000003</v>
       </c>
-      <c r="I20" s="102">
+      <c r="I20" s="64">
         <v>3054</v>
       </c>
-      <c r="J20" s="83"/>
-      <c r="K20" s="106">
+      <c r="J20" s="66"/>
+      <c r="K20" s="70">
         <v>0</v>
       </c>
-      <c r="L20" s="105">
+      <c r="L20" s="82">
         <v>0</v>
       </c>
-      <c r="M20" s="105">
+      <c r="M20" s="82">
         <v>0</v>
       </c>
-      <c r="N20" s="102">
+      <c r="N20" s="64">
         <v>46</v>
       </c>
       <c r="O20" s="27"/>
     </row>
     <row r="21" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
-      <c r="B21" s="101"/>
-      <c r="C21" s="102" t="s">
+      <c r="B21" s="98"/>
+      <c r="C21" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="102" t="s">
+      <c r="D21" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="103"/>
-      <c r="F21" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="G21" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="H21" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="I21" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="J21" s="83"/>
-      <c r="K21" s="105">
+      <c r="E21" s="65"/>
+      <c r="F21" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="J21" s="66"/>
+      <c r="K21" s="82">
         <v>4.2666999999999997E-2</v>
       </c>
-      <c r="L21" s="105">
+      <c r="L21" s="82">
         <v>0.34782600000000002</v>
       </c>
-      <c r="M21" s="105">
+      <c r="M21" s="82">
         <v>7.6009999999999994E-2</v>
       </c>
-      <c r="N21" s="102">
+      <c r="N21" s="64">
         <v>46</v>
       </c>
       <c r="O21" s="27"/>
     </row>
     <row r="22" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="27"/>
-      <c r="B22" s="101"/>
-      <c r="C22" s="102" t="s">
+      <c r="B22" s="98"/>
+      <c r="C22" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="102" t="s">
+      <c r="D22" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="103"/>
-      <c r="F22" s="106">
+      <c r="E22" s="65"/>
+      <c r="F22" s="70">
         <v>0.171429</v>
       </c>
-      <c r="G22" s="106">
+      <c r="G22" s="70">
         <v>0.259459</v>
       </c>
-      <c r="H22" s="106">
+      <c r="H22" s="70">
         <v>0.206452</v>
       </c>
-      <c r="I22" s="102">
+      <c r="I22" s="64">
         <v>185</v>
       </c>
-      <c r="J22" s="83"/>
-      <c r="K22" s="105">
+      <c r="J22" s="66"/>
+      <c r="K22" s="82">
         <v>0.36082500000000001</v>
       </c>
-      <c r="L22" s="105">
+      <c r="L22" s="82">
         <v>0.12302299999999999</v>
       </c>
-      <c r="M22" s="105">
+      <c r="M22" s="82">
         <v>0.18348600000000001</v>
       </c>
-      <c r="N22" s="102">
+      <c r="N22" s="64">
         <v>569</v>
       </c>
       <c r="O22" s="27"/>
     </row>
     <row r="23" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
-      <c r="B23" s="101"/>
-      <c r="C23" s="102" t="s">
+      <c r="B23" s="98"/>
+      <c r="C23" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="102" t="s">
+      <c r="D23" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="103"/>
-      <c r="F23" s="106">
+      <c r="E23" s="65"/>
+      <c r="F23" s="70">
         <v>5.9563999999999999E-2</v>
       </c>
-      <c r="G23" s="106">
+      <c r="G23" s="70">
         <v>0.27734399999999998</v>
       </c>
-      <c r="H23" s="106">
+      <c r="H23" s="70">
         <v>9.8066E-2</v>
       </c>
-      <c r="I23" s="102">
+      <c r="I23" s="64">
         <v>256</v>
       </c>
-      <c r="J23" s="83"/>
-      <c r="K23" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="L23" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="M23" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="N23" s="102" t="s">
+      <c r="J23" s="66"/>
+      <c r="K23" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="L23" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="M23" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="N23" s="64" t="s">
         <v>80</v>
       </c>
       <c r="O23" s="27"/>
     </row>
     <row r="24" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
-      <c r="B24" s="101"/>
-      <c r="C24" s="91" t="s">
+      <c r="B24" s="98"/>
+      <c r="C24" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="91" t="s">
+      <c r="D24" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="92"/>
-      <c r="F24" s="107">
+      <c r="E24" s="74"/>
+      <c r="F24" s="83">
         <v>3.3333000000000002E-2</v>
       </c>
-      <c r="G24" s="93">
+      <c r="G24" s="75">
         <v>8.6580000000000004E-2</v>
       </c>
-      <c r="H24" s="107">
+      <c r="H24" s="83">
         <v>4.8134999999999997E-2</v>
       </c>
-      <c r="I24" s="91">
+      <c r="I24" s="73">
         <v>231</v>
       </c>
-      <c r="J24" s="94"/>
-      <c r="K24" s="107">
+      <c r="J24" s="76"/>
+      <c r="K24" s="83">
         <v>0.44444400000000001</v>
       </c>
-      <c r="L24" s="107">
+      <c r="L24" s="83">
         <v>0.122123</v>
       </c>
-      <c r="M24" s="107">
+      <c r="M24" s="83">
         <v>0.19159899999999999</v>
       </c>
-      <c r="N24" s="91">
+      <c r="N24" s="73">
         <v>2129</v>
       </c>
       <c r="O24" s="27"/>
     </row>
     <row r="25" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="27"/>
-      <c r="B25" s="108"/>
-      <c r="C25" s="109" t="s">
+      <c r="B25" s="84"/>
+      <c r="C25" s="97" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="109"/>
-      <c r="E25" s="109"/>
-      <c r="F25" s="110">
+      <c r="D25" s="97"/>
+      <c r="E25" s="97"/>
+      <c r="F25" s="107">
         <v>0.6129</v>
       </c>
-      <c r="G25" s="110"/>
-      <c r="H25" s="110"/>
-      <c r="I25" s="110"/>
-      <c r="J25" s="111"/>
-      <c r="K25" s="110">
+      <c r="G25" s="107"/>
+      <c r="H25" s="107"/>
+      <c r="I25" s="107"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="107">
         <v>0.76049999999999995</v>
       </c>
-      <c r="L25" s="110"/>
-      <c r="M25" s="110"/>
-      <c r="N25" s="110"/>
+      <c r="L25" s="107"/>
+      <c r="M25" s="107"/>
+      <c r="N25" s="107"/>
       <c r="O25" s="27"/>
     </row>
     <row r="26" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
-      <c r="B26" s="112" t="s">
+      <c r="B26" s="105" t="s">
         <v>112</v>
       </c>
-      <c r="C26" s="112"/>
-      <c r="D26" s="112"/>
-      <c r="E26" s="112"/>
-      <c r="F26" s="112"/>
-      <c r="G26" s="112"/>
-      <c r="H26" s="112"/>
-      <c r="I26" s="112"/>
-      <c r="J26" s="112"/>
-      <c r="K26" s="112"/>
-      <c r="L26" s="112"/>
-      <c r="M26" s="112"/>
-      <c r="N26" s="112"/>
+      <c r="C26" s="105"/>
+      <c r="D26" s="105"/>
+      <c r="E26" s="105"/>
+      <c r="F26" s="105"/>
+      <c r="G26" s="105"/>
+      <c r="H26" s="105"/>
+      <c r="I26" s="105"/>
+      <c r="J26" s="105"/>
+      <c r="K26" s="105"/>
+      <c r="L26" s="105"/>
+      <c r="M26" s="105"/>
+      <c r="N26" s="105"/>
       <c r="O26" s="27"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="22"/>
       <c r="B27" s="22"/>
       <c r="C27" s="25"/>
-      <c r="D27" s="67"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="23"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
@@ -2796,17 +2847,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B15:B24"/>
-    <mergeCell ref="B4:B13"/>
-    <mergeCell ref="F2:I2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="B26:N26"/>
     <mergeCell ref="K14:N14"/>
     <mergeCell ref="F14:I14"/>
     <mergeCell ref="F25:I25"/>
     <mergeCell ref="K25:N25"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="B15:B24"/>
+    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2854,19 +2905,19 @@
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="61" t="s">
+      <c r="E2" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="63"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="113"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="61" t="s">
+      <c r="J2" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="63"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="112"/>
+      <c r="M2" s="113"/>
       <c r="N2" s="27"/>
     </row>
     <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2909,7 +2960,7 @@
     </row>
     <row r="4" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="27"/>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="109" t="s">
         <v>111</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -2947,7 +2998,7 @@
     </row>
     <row r="5" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27"/>
-      <c r="B5" s="59"/>
+      <c r="B5" s="109"/>
       <c r="C5" s="7" t="s">
         <v>18</v>
       </c>
@@ -2983,7 +3034,7 @@
     </row>
     <row r="6" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
-      <c r="B6" s="59"/>
+      <c r="B6" s="109"/>
       <c r="C6" s="7" t="s">
         <v>1</v>
       </c>
@@ -3019,7 +3070,7 @@
     </row>
     <row r="7" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
-      <c r="B7" s="59"/>
+      <c r="B7" s="109"/>
       <c r="C7" s="7" t="s">
         <v>2</v>
       </c>
@@ -3055,7 +3106,7 @@
     </row>
     <row r="8" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
-      <c r="B8" s="59"/>
+      <c r="B8" s="109"/>
       <c r="C8" s="7" t="s">
         <v>7</v>
       </c>
@@ -3091,7 +3142,7 @@
     </row>
     <row r="9" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="59"/>
+      <c r="B9" s="109"/>
       <c r="C9" s="7" t="s">
         <v>3</v>
       </c>
@@ -3127,7 +3178,7 @@
     </row>
     <row r="10" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
-      <c r="B10" s="59"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
@@ -3163,7 +3214,7 @@
     </row>
     <row r="11" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
-      <c r="B11" s="59"/>
+      <c r="B11" s="109"/>
       <c r="C11" s="7" t="s">
         <v>5</v>
       </c>
@@ -3199,7 +3250,7 @@
     </row>
     <row r="12" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
-      <c r="B12" s="59"/>
+      <c r="B12" s="109"/>
       <c r="C12" s="7" t="s">
         <v>4</v>
       </c>
@@ -3235,7 +3286,7 @@
     </row>
     <row r="13" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
-      <c r="B13" s="59"/>
+      <c r="B13" s="109"/>
       <c r="C13" s="7" t="s">
         <v>6</v>
       </c>
@@ -3271,7 +3322,7 @@
     </row>
     <row r="14" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
-      <c r="B14" s="59"/>
+      <c r="B14" s="109"/>
       <c r="C14" s="41" t="s">
         <v>93</v>
       </c>
@@ -3293,23 +3344,23 @@
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
-      <c r="B15" s="64"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="65"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="114"/>
+      <c r="D15" s="114"/>
+      <c r="E15" s="114"/>
+      <c r="F15" s="114"/>
+      <c r="G15" s="114"/>
+      <c r="H15" s="114"/>
+      <c r="I15" s="114"/>
+      <c r="J15" s="114"/>
+      <c r="K15" s="114"/>
+      <c r="L15" s="114"/>
+      <c r="M15" s="114"/>
       <c r="N15" s="27"/>
     </row>
     <row r="16" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="109" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -3347,7 +3398,7 @@
     </row>
     <row r="17" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27"/>
-      <c r="B17" s="59"/>
+      <c r="B17" s="109"/>
       <c r="C17" s="7" t="s">
         <v>18</v>
       </c>
@@ -3383,7 +3434,7 @@
     </row>
     <row r="18" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
-      <c r="B18" s="59"/>
+      <c r="B18" s="109"/>
       <c r="C18" s="7" t="s">
         <v>1</v>
       </c>
@@ -3419,7 +3470,7 @@
     </row>
     <row r="19" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
-      <c r="B19" s="59"/>
+      <c r="B19" s="109"/>
       <c r="C19" s="7" t="s">
         <v>2</v>
       </c>
@@ -3455,7 +3506,7 @@
     </row>
     <row r="20" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
-      <c r="B20" s="59"/>
+      <c r="B20" s="109"/>
       <c r="C20" s="7" t="s">
         <v>7</v>
       </c>
@@ -3491,7 +3542,7 @@
     </row>
     <row r="21" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
-      <c r="B21" s="59"/>
+      <c r="B21" s="109"/>
       <c r="C21" s="7" t="s">
         <v>3</v>
       </c>
@@ -3527,7 +3578,7 @@
     </row>
     <row r="22" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="27"/>
-      <c r="B22" s="59"/>
+      <c r="B22" s="109"/>
       <c r="C22" s="7" t="s">
         <v>17</v>
       </c>
@@ -3563,7 +3614,7 @@
     </row>
     <row r="23" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
-      <c r="B23" s="59"/>
+      <c r="B23" s="109"/>
       <c r="C23" s="7" t="s">
         <v>5</v>
       </c>
@@ -3599,7 +3650,7 @@
     </row>
     <row r="24" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
-      <c r="B24" s="59"/>
+      <c r="B24" s="109"/>
       <c r="C24" s="7" t="s">
         <v>4</v>
       </c>
@@ -3635,7 +3686,7 @@
     </row>
     <row r="25" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
-      <c r="B25" s="59"/>
+      <c r="B25" s="109"/>
       <c r="C25" s="7" t="s">
         <v>6</v>
       </c>
@@ -3671,7 +3722,7 @@
     </row>
     <row r="26" spans="1:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
-      <c r="B26" s="60"/>
+      <c r="B26" s="110"/>
       <c r="C26" s="49" t="s">
         <v>93</v>
       </c>
@@ -3693,20 +3744,20 @@
     </row>
     <row r="27" spans="1:14" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
-      <c r="B27" s="58" t="s">
+      <c r="B27" s="108" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="58"/>
-      <c r="J27" s="58"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="58"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="108"/>
+      <c r="F27" s="108"/>
+      <c r="G27" s="108"/>
+      <c r="H27" s="108"/>
+      <c r="I27" s="108"/>
+      <c r="J27" s="108"/>
+      <c r="K27" s="108"/>
+      <c r="L27" s="108"/>
+      <c r="M27" s="108"/>
       <c r="N27" s="27"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -3746,7 +3797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1082DB7A-7957-7A42-9B70-00DEB116BD14}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G17"/>
     </sheetView>
   </sheetViews>
@@ -3761,402 +3812,402 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="58" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="113" t="s">
+      <c r="C1" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="113" t="s">
+      <c r="D1" s="86" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="113" t="s">
+      <c r="E1" s="86" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="113" t="s">
+      <c r="F1" s="86" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="113" t="s">
+      <c r="G1" s="86" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="118">
+      <c r="C2" s="91">
         <v>220.27506549909401</v>
       </c>
-      <c r="D2" s="118">
+      <c r="D2" s="91">
         <v>334.69343574769903</v>
       </c>
-      <c r="E2" s="118">
+      <c r="E2" s="91">
         <v>15.382730846667</v>
       </c>
-      <c r="F2" s="118">
+      <c r="F2" s="91">
         <v>21.930870636858302</v>
       </c>
-      <c r="G2" s="118">
+      <c r="G2" s="91">
         <v>26.629367653239399</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="118">
+      <c r="C3" s="91">
         <v>379.31745140005103</v>
       </c>
-      <c r="D3" s="118">
+      <c r="D3" s="91">
         <v>590.03648386146006</v>
       </c>
-      <c r="E3" s="118">
+      <c r="E3" s="91">
         <v>21.179419316919098</v>
       </c>
-      <c r="F3" s="118">
+      <c r="F3" s="91">
         <v>34.7890294337437</v>
       </c>
-      <c r="G3" s="118">
+      <c r="G3" s="91">
         <v>44.489682577496502</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="118">
+      <c r="C4" s="91">
         <v>95.621198596277395</v>
       </c>
-      <c r="D4" s="118">
+      <c r="D4" s="91">
         <v>166.17011075683899</v>
       </c>
-      <c r="E4" s="119">
+      <c r="E4" s="92">
         <v>9.8315021210795894</v>
       </c>
-      <c r="F4" s="118">
+      <c r="F4" s="91">
         <v>17.7557434722859</v>
       </c>
-      <c r="G4" s="118">
+      <c r="G4" s="91">
         <v>14.1942713916334</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="118">
+      <c r="C5" s="91">
         <v>173.86908530727999</v>
       </c>
-      <c r="D5" s="118">
+      <c r="D5" s="91">
         <v>255.85089025534501</v>
       </c>
-      <c r="E5" s="119">
+      <c r="E5" s="92">
         <v>13.5642210617237</v>
       </c>
-      <c r="F5" s="118">
+      <c r="F5" s="91">
         <v>20.190239248841099</v>
       </c>
-      <c r="G5" s="118">
+      <c r="G5" s="91">
         <v>20.549340032271701</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="102" t="s">
+      <c r="A6" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="102" t="s">
+      <c r="B6" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="118">
+      <c r="C6" s="91">
         <v>82.708314592231702</v>
       </c>
-      <c r="D6" s="118">
+      <c r="D6" s="91">
         <v>116.70004006871601</v>
       </c>
-      <c r="E6" s="118">
+      <c r="E6" s="91">
         <v>10.0221515488718</v>
       </c>
-      <c r="F6" s="118">
+      <c r="F6" s="91">
         <v>19.884409272063401</v>
       </c>
-      <c r="G6" s="118">
+      <c r="G6" s="91">
         <v>8.7993093645175993</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="102" t="s">
+      <c r="B7" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="118">
+      <c r="C7" s="91">
         <v>104.68908088121201</v>
       </c>
-      <c r="D7" s="118">
+      <c r="D7" s="91">
         <v>182.13219334494499</v>
       </c>
-      <c r="E7" s="118">
+      <c r="E7" s="91">
         <v>10.5693738694885</v>
       </c>
-      <c r="F7" s="118">
+      <c r="F7" s="91">
         <v>19.021785327102702</v>
       </c>
-      <c r="G7" s="118">
+      <c r="G7" s="91">
         <v>71.354922104783597</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="102" t="s">
+      <c r="A8" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="102" t="s">
+      <c r="B8" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="118">
+      <c r="C8" s="91">
         <v>107.886702988707</v>
       </c>
-      <c r="D8" s="118">
+      <c r="D8" s="91">
         <v>184.171685382558</v>
       </c>
-      <c r="E8" s="118">
+      <c r="E8" s="91">
         <v>10.6488204660593</v>
       </c>
-      <c r="F8" s="118">
+      <c r="F8" s="91">
         <v>19.044169978669</v>
       </c>
-      <c r="G8" s="118">
+      <c r="G8" s="91">
         <v>18.755446237862099</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="102" t="s">
+      <c r="A9" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="102" t="s">
+      <c r="B9" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="118">
+      <c r="C9" s="91">
         <v>542.68229075136003</v>
       </c>
-      <c r="D9" s="118">
+      <c r="D9" s="91">
         <v>1027.8829639800599</v>
       </c>
-      <c r="E9" s="118">
+      <c r="E9" s="91">
         <v>27.1057496126442</v>
       </c>
-      <c r="F9" s="118">
+      <c r="F9" s="91">
         <v>54.098619200023499</v>
       </c>
-      <c r="G9" s="118">
+      <c r="G9" s="91">
         <v>214.80549647180499</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="102" t="s">
+      <c r="A10" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="102" t="s">
+      <c r="B10" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="118">
+      <c r="C10" s="91">
         <v>498.94227236199498</v>
       </c>
-      <c r="D10" s="118">
+      <c r="D10" s="91">
         <v>824.95648802397398</v>
       </c>
-      <c r="E10" s="118">
+      <c r="E10" s="91">
         <v>22.7507241660383</v>
       </c>
-      <c r="F10" s="118">
+      <c r="F10" s="91">
         <v>49.078231056572399</v>
       </c>
-      <c r="G10" s="118">
+      <c r="G10" s="91">
         <v>175.87511521959601</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="102" t="s">
+      <c r="A11" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="102" t="s">
+      <c r="B11" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="118">
+      <c r="C11" s="91">
         <v>126.227110773001</v>
       </c>
-      <c r="D11" s="118">
+      <c r="D11" s="91">
         <v>222.33527165872101</v>
       </c>
-      <c r="E11" s="118">
+      <c r="E11" s="91">
         <v>11.5062202643132</v>
       </c>
-      <c r="F11" s="118">
+      <c r="F11" s="91">
         <v>20.643445573906501</v>
       </c>
-      <c r="G11" s="118">
+      <c r="G11" s="91">
         <v>48.873946613739598</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="102" t="s">
+      <c r="A12" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="102" t="s">
+      <c r="B12" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="118">
+      <c r="C12" s="91">
         <v>261.38382021655798</v>
       </c>
-      <c r="D12" s="118">
+      <c r="D12" s="91">
         <v>440.40977483692598</v>
       </c>
-      <c r="E12" s="118">
+      <c r="E12" s="91">
         <v>16.510694774972301</v>
       </c>
-      <c r="F12" s="118">
+      <c r="F12" s="91">
         <v>26.692685260847401</v>
       </c>
-      <c r="G12" s="118">
+      <c r="G12" s="91">
         <v>63.599778794705998</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="102" t="s">
+      <c r="A13" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="102" t="s">
+      <c r="B13" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C13" s="118">
+      <c r="C13" s="91">
         <v>87.148012158031193</v>
       </c>
-      <c r="D13" s="118">
+      <c r="D13" s="91">
         <v>117.24957666139601</v>
       </c>
-      <c r="E13" s="118">
+      <c r="E13" s="91">
         <v>10.512395000826601</v>
       </c>
-      <c r="F13" s="118">
+      <c r="F13" s="91">
         <v>20.7658764592904</v>
       </c>
-      <c r="G13" s="118">
+      <c r="G13" s="91">
         <v>29.033984653242399</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="102" t="s">
+      <c r="A14" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="102" t="s">
+      <c r="B14" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="118">
+      <c r="C14" s="91">
         <v>109.261167023997</v>
       </c>
-      <c r="D14" s="118">
+      <c r="D14" s="91">
         <v>212.27639757314699</v>
       </c>
-      <c r="E14" s="118">
+      <c r="E14" s="91">
         <v>10.588381463307501</v>
       </c>
-      <c r="F14" s="118">
+      <c r="F14" s="91">
         <v>19.0095787584211</v>
       </c>
-      <c r="G14" s="118">
+      <c r="G14" s="91">
         <v>50.882362019531797</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="114" t="s">
+      <c r="A15" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="114" t="s">
+      <c r="B15" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="120">
+      <c r="C15" s="93">
         <v>250.79733709748501</v>
       </c>
-      <c r="D15" s="120">
+      <c r="D15" s="93">
         <v>393.92710490360201</v>
       </c>
-      <c r="E15" s="121">
+      <c r="E15" s="94">
         <v>16.6929243566304</v>
       </c>
-      <c r="F15" s="120">
+      <c r="F15" s="93">
         <v>27.523993624934501</v>
       </c>
-      <c r="G15" s="120">
+      <c r="G15" s="93">
         <v>44.5767797935586</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="115" t="s">
+      <c r="A16" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="122">
+      <c r="C16" s="92">
         <f>AVERAGE(C2:C3,C5,C9,C10,C12,C15)</f>
         <v>332.46676037626042</v>
       </c>
-      <c r="D16" s="122">
+      <c r="D16" s="92">
         <f>AVERAGE(D2:D3,D5,D9,D10,D12,D15)</f>
         <v>552.53673451558086</v>
       </c>
-      <c r="E16" s="122">
+      <c r="E16" s="92">
         <f t="shared" ref="E16:G16" si="0">AVERAGE(E2:E3,E5,E9,E10,E12,E15)</f>
         <v>19.026637733656425</v>
       </c>
-      <c r="F16" s="122">
+      <c r="F16" s="92">
         <f t="shared" si="0"/>
         <v>33.471952637402985</v>
       </c>
-      <c r="G16" s="122">
+      <c r="G16" s="92">
         <f t="shared" si="0"/>
         <v>84.360794363239023</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="116" t="s">
+      <c r="A17" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="117" t="s">
+      <c r="B17" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="123">
+      <c r="C17" s="95">
         <f>AVERAGE(C4,C6,C7,C8,C11,C13,C14)</f>
         <v>101.9345124304939</v>
       </c>
-      <c r="D17" s="123">
+      <c r="D17" s="95">
         <f t="shared" ref="D17:G17" si="1">AVERAGE(D4,D6,D7,D8,D11,D13,D14)</f>
         <v>171.57646792090313</v>
       </c>
-      <c r="E17" s="123">
+      <c r="E17" s="95">
         <f t="shared" si="1"/>
         <v>10.525549247706641</v>
       </c>
-      <c r="F17" s="123">
+      <c r="F17" s="95">
         <f t="shared" si="1"/>
         <v>19.446429834534143</v>
       </c>
-      <c r="G17" s="123">
+      <c r="G17" s="95">
         <f t="shared" si="1"/>
         <v>34.556320340758639</v>
       </c>
@@ -4188,508 +4239,508 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="58" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="113" t="s">
+      <c r="C1" s="86" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="113" t="s">
+      <c r="D1" s="86" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="113" t="s">
+      <c r="E1" s="86" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="113" t="s">
+      <c r="F1" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="113" t="s">
+      <c r="G1" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="113" t="s">
+      <c r="H1" s="86" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="113" t="s">
+      <c r="I1" s="86" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="118">
+      <c r="C2" s="91">
         <v>220.27506549909401</v>
       </c>
-      <c r="D2" s="118">
+      <c r="D2" s="91">
         <v>334.69343574769903</v>
       </c>
-      <c r="E2" s="118">
+      <c r="E2" s="91">
         <v>15.382730846667</v>
       </c>
-      <c r="F2" s="118">
+      <c r="F2" s="91">
         <v>2.0967558483962301</v>
       </c>
-      <c r="G2" s="118">
+      <c r="G2" s="91">
         <v>139.57570602561401</v>
       </c>
-      <c r="H2" s="118">
+      <c r="H2" s="91">
         <v>21.930870636858302</v>
       </c>
-      <c r="I2" s="118">
+      <c r="I2" s="91">
         <v>26.629367653239399</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="118">
+      <c r="C3" s="91">
         <v>379.31745140005103</v>
       </c>
-      <c r="D3" s="118">
+      <c r="D3" s="91">
         <v>590.03648386146006</v>
       </c>
-      <c r="E3" s="118">
+      <c r="E3" s="91">
         <v>21.179419316919098</v>
       </c>
-      <c r="F3" s="118">
+      <c r="F3" s="91">
         <v>3.24925095739661</v>
       </c>
-      <c r="G3" s="118">
+      <c r="G3" s="91">
         <v>86.199472639969201</v>
       </c>
-      <c r="H3" s="118">
+      <c r="H3" s="91">
         <v>34.7890294337437</v>
       </c>
-      <c r="I3" s="118">
+      <c r="I3" s="91">
         <v>44.489682577496502</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="118">
+      <c r="C4" s="91">
         <v>95.621198596277395</v>
       </c>
-      <c r="D4" s="118">
+      <c r="D4" s="91">
         <v>166.17011075683899</v>
       </c>
-      <c r="E4" s="119">
+      <c r="E4" s="92">
         <v>9.8315021210795894</v>
       </c>
-      <c r="F4" s="118">
+      <c r="F4" s="91">
         <v>2.2727192059350698</v>
       </c>
-      <c r="G4" s="118">
+      <c r="G4" s="91">
         <v>173.028615917434</v>
       </c>
-      <c r="H4" s="118">
+      <c r="H4" s="91">
         <v>17.7557434722859</v>
       </c>
-      <c r="I4" s="118">
+      <c r="I4" s="91">
         <v>14.1942713916334</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="118">
+      <c r="C5" s="91">
         <v>173.86908530727999</v>
       </c>
-      <c r="D5" s="118">
+      <c r="D5" s="91">
         <v>255.85089025534501</v>
       </c>
-      <c r="E5" s="119">
+      <c r="E5" s="92">
         <v>13.5642210617237</v>
       </c>
-      <c r="F5" s="118">
+      <c r="F5" s="91">
         <v>2.0210238278750201</v>
       </c>
-      <c r="G5" s="118">
+      <c r="G5" s="91">
         <v>137.451338394381</v>
       </c>
-      <c r="H5" s="118">
+      <c r="H5" s="91">
         <v>20.190239248841099</v>
       </c>
-      <c r="I5" s="118">
+      <c r="I5" s="91">
         <v>20.549340032271701</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="102" t="s">
+      <c r="A6" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="102" t="s">
+      <c r="B6" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="118">
+      <c r="C6" s="91">
         <v>82.708314592231702</v>
       </c>
-      <c r="D6" s="118">
+      <c r="D6" s="91">
         <v>116.70004006871601</v>
       </c>
-      <c r="E6" s="118">
+      <c r="E6" s="91">
         <v>10.0221515488718</v>
       </c>
-      <c r="F6" s="118">
+      <c r="F6" s="91">
         <v>4.1433372422797303</v>
       </c>
-      <c r="G6" s="118">
+      <c r="G6" s="91">
         <v>125.457655935356</v>
       </c>
-      <c r="H6" s="118">
+      <c r="H6" s="91">
         <v>19.884409272063401</v>
       </c>
-      <c r="I6" s="118">
+      <c r="I6" s="91">
         <v>8.7993093645175993</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="102" t="s">
+      <c r="B7" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="118">
+      <c r="C7" s="91">
         <v>104.68908088121201</v>
       </c>
-      <c r="D7" s="118">
+      <c r="D7" s="91">
         <v>182.13219334494499</v>
       </c>
-      <c r="E7" s="118">
+      <c r="E7" s="91">
         <v>10.5693738694885</v>
       </c>
-      <c r="F7" s="119">
+      <c r="F7" s="92">
         <v>2.7643741084442301</v>
       </c>
-      <c r="G7" s="118">
+      <c r="G7" s="91">
         <v>57.38189647438</v>
       </c>
-      <c r="H7" s="118">
+      <c r="H7" s="91">
         <v>19.021785327102702</v>
       </c>
-      <c r="I7" s="118">
+      <c r="I7" s="91">
         <v>71.354922104783597</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="102" t="s">
+      <c r="A8" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="102" t="s">
+      <c r="B8" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="118">
+      <c r="C8" s="91">
         <v>107.886702988707</v>
       </c>
-      <c r="D8" s="118">
+      <c r="D8" s="91">
         <v>184.171685382558</v>
       </c>
-      <c r="E8" s="118">
+      <c r="E8" s="91">
         <v>10.6488204660593</v>
       </c>
-      <c r="F8" s="118">
+      <c r="F8" s="91">
         <v>2.01997989498062</v>
       </c>
-      <c r="G8" s="118">
+      <c r="G8" s="91">
         <v>125.562192674638</v>
       </c>
-      <c r="H8" s="118">
+      <c r="H8" s="91">
         <v>19.044169978669</v>
       </c>
-      <c r="I8" s="118">
+      <c r="I8" s="91">
         <v>18.755446237862099</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="102" t="s">
+      <c r="A9" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="102" t="s">
+      <c r="B9" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="118">
+      <c r="C9" s="91">
         <v>542.68229075136003</v>
       </c>
-      <c r="D9" s="118">
+      <c r="D9" s="91">
         <v>1027.8829639800599</v>
       </c>
-      <c r="E9" s="118">
+      <c r="E9" s="91">
         <v>27.1057496126442</v>
       </c>
-      <c r="F9" s="118">
+      <c r="F9" s="91">
         <v>5.3485585945545502</v>
       </c>
-      <c r="G9" s="118">
+      <c r="G9" s="91">
         <v>95.974985206733905</v>
       </c>
-      <c r="H9" s="118">
+      <c r="H9" s="91">
         <v>54.098619200023499</v>
       </c>
-      <c r="I9" s="118">
+      <c r="I9" s="91">
         <v>214.80549647180499</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="102" t="s">
+      <c r="A10" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="102" t="s">
+      <c r="B10" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="118">
+      <c r="C10" s="91">
         <v>498.94227236199498</v>
       </c>
-      <c r="D10" s="118">
+      <c r="D10" s="91">
         <v>824.95648802397398</v>
       </c>
-      <c r="E10" s="118">
+      <c r="E10" s="91">
         <v>22.7507241660383</v>
       </c>
-      <c r="F10" s="118">
+      <c r="F10" s="91">
         <v>6.634754757204</v>
       </c>
-      <c r="G10" s="118">
+      <c r="G10" s="91">
         <v>228.912870683872</v>
       </c>
-      <c r="H10" s="118">
+      <c r="H10" s="91">
         <v>49.078231056572399</v>
       </c>
-      <c r="I10" s="118">
+      <c r="I10" s="91">
         <v>175.87511521959601</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="102" t="s">
+      <c r="A11" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="102" t="s">
+      <c r="B11" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="118">
+      <c r="C11" s="91">
         <v>126.227110773001</v>
       </c>
-      <c r="D11" s="118">
+      <c r="D11" s="91">
         <v>222.33527165872101</v>
       </c>
-      <c r="E11" s="118">
+      <c r="E11" s="91">
         <v>11.5062202643132</v>
       </c>
-      <c r="F11" s="118">
+      <c r="F11" s="91">
         <v>2.41072168645512</v>
       </c>
-      <c r="G11" s="118">
+      <c r="G11" s="91">
         <v>118.610064263905</v>
       </c>
-      <c r="H11" s="118">
+      <c r="H11" s="91">
         <v>20.643445573906501</v>
       </c>
-      <c r="I11" s="118">
+      <c r="I11" s="91">
         <v>48.873946613739598</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="102" t="s">
+      <c r="A12" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="102" t="s">
+      <c r="B12" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="118">
+      <c r="C12" s="91">
         <v>261.38382021655798</v>
       </c>
-      <c r="D12" s="118">
+      <c r="D12" s="91">
         <v>440.40977483692598</v>
       </c>
-      <c r="E12" s="118">
+      <c r="E12" s="91">
         <v>16.510694774972301</v>
       </c>
-      <c r="F12" s="118">
+      <c r="F12" s="91">
         <v>2.2807164493294101</v>
       </c>
-      <c r="G12" s="119">
+      <c r="G12" s="92">
         <v>102.425393598171</v>
       </c>
-      <c r="H12" s="118">
+      <c r="H12" s="91">
         <v>26.692685260847401</v>
       </c>
-      <c r="I12" s="118">
+      <c r="I12" s="91">
         <v>63.599778794705998</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="102" t="s">
+      <c r="A13" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="102" t="s">
+      <c r="B13" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C13" s="118">
+      <c r="C13" s="91">
         <v>87.148012158031193</v>
       </c>
-      <c r="D13" s="118">
+      <c r="D13" s="91">
         <v>117.24957666139601</v>
       </c>
-      <c r="E13" s="118">
+      <c r="E13" s="91">
         <v>10.512395000826601</v>
       </c>
-      <c r="F13" s="118">
+      <c r="F13" s="91">
         <v>4.6426125936193197</v>
       </c>
-      <c r="G13" s="119">
+      <c r="G13" s="92">
         <v>74.499673476889399</v>
       </c>
-      <c r="H13" s="118">
+      <c r="H13" s="91">
         <v>20.7658764592904</v>
       </c>
-      <c r="I13" s="118">
+      <c r="I13" s="91">
         <v>29.033984653242399</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="102" t="s">
+      <c r="A14" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="102" t="s">
+      <c r="B14" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="118">
+      <c r="C14" s="91">
         <v>109.261167023997</v>
       </c>
-      <c r="D14" s="118">
+      <c r="D14" s="91">
         <v>212.27639757314699</v>
       </c>
-      <c r="E14" s="118">
+      <c r="E14" s="91">
         <v>10.588381463307501</v>
       </c>
-      <c r="F14" s="118">
+      <c r="F14" s="91">
         <v>2.2051777612235002</v>
       </c>
-      <c r="G14" s="118">
+      <c r="G14" s="91">
         <v>47.657607673278498</v>
       </c>
-      <c r="H14" s="118">
+      <c r="H14" s="91">
         <v>19.0095787584211</v>
       </c>
-      <c r="I14" s="118">
+      <c r="I14" s="91">
         <v>50.882362019531797</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="114" t="s">
+      <c r="A15" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="114" t="s">
+      <c r="B15" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="120">
+      <c r="C15" s="93">
         <v>250.79733709748501</v>
       </c>
-      <c r="D15" s="120">
+      <c r="D15" s="93">
         <v>393.92710490360201</v>
       </c>
-      <c r="E15" s="121">
+      <c r="E15" s="94">
         <v>16.6929243566304</v>
       </c>
-      <c r="F15" s="120">
+      <c r="F15" s="93">
         <v>2.5984820585417299</v>
       </c>
-      <c r="G15" s="121">
+      <c r="G15" s="94">
         <v>70.665041237155407</v>
       </c>
-      <c r="H15" s="120">
+      <c r="H15" s="93">
         <v>27.523993624934501</v>
       </c>
-      <c r="I15" s="120">
+      <c r="I15" s="93">
         <v>44.5767797935586</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="115" t="s">
+      <c r="A16" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="122">
+      <c r="C16" s="92">
         <f>AVERAGE(C2:C3,C5,C9,C10,C12,C15)</f>
         <v>332.46676037626042</v>
       </c>
-      <c r="D16" s="122">
+      <c r="D16" s="92">
         <f>AVERAGE(D2:D3,D5,D9,D10,D12,D15)</f>
         <v>552.53673451558086</v>
       </c>
-      <c r="E16" s="122">
+      <c r="E16" s="92">
         <f t="shared" ref="E16:I16" si="0">AVERAGE(E2:E3,E5,E9,E10,E12,E15)</f>
         <v>19.026637733656425</v>
       </c>
-      <c r="F16" s="122">
+      <c r="F16" s="92">
         <f t="shared" si="0"/>
         <v>3.4613632133282217</v>
       </c>
-      <c r="G16" s="122">
+      <c r="G16" s="92">
         <f t="shared" si="0"/>
         <v>123.02925825512807</v>
       </c>
-      <c r="H16" s="122">
+      <c r="H16" s="92">
         <f t="shared" si="0"/>
         <v>33.471952637402985</v>
       </c>
-      <c r="I16" s="122">
+      <c r="I16" s="92">
         <f t="shared" si="0"/>
         <v>84.360794363239023</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="116" t="s">
+      <c r="A17" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="117" t="s">
+      <c r="B17" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="123">
+      <c r="C17" s="95">
         <f>AVERAGE(C4,C6,C7,C8,C11,C13,C14)</f>
         <v>101.9345124304939</v>
       </c>
-      <c r="D17" s="123">
+      <c r="D17" s="95">
         <f t="shared" ref="D17:I17" si="1">AVERAGE(D4,D6,D7,D8,D11,D13,D14)</f>
         <v>171.57646792090313</v>
       </c>
-      <c r="E17" s="123">
+      <c r="E17" s="95">
         <f t="shared" si="1"/>
         <v>10.525549247706641</v>
       </c>
-      <c r="F17" s="123">
+      <c r="F17" s="95">
         <f t="shared" si="1"/>
         <v>2.9227032132767983</v>
       </c>
-      <c r="G17" s="123">
+      <c r="G17" s="95">
         <f t="shared" si="1"/>
         <v>103.17110091655441</v>
       </c>
-      <c r="H17" s="123">
+      <c r="H17" s="95">
         <f t="shared" si="1"/>
         <v>19.446429834534143</v>
       </c>
-      <c r="I17" s="123">
+      <c r="I17" s="95">
         <f t="shared" si="1"/>
         <v>34.556320340758639</v>
       </c>
@@ -4698,4 +4749,425 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577482D8-1285-B642-9F2B-8A4300CFC9C7}">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13:H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" customWidth="1"/>
+    <col min="7" max="10" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="130"/>
+      <c r="B1" s="128" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="128" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+    </row>
+    <row r="2" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="127" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="126" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="126" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="126" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="126" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="126" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="125" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="125"/>
+      <c r="G3" s="124">
+        <v>0.82168200000000002</v>
+      </c>
+      <c r="H3" s="124">
+        <v>0.96934100000000001</v>
+      </c>
+      <c r="I3" s="124">
+        <v>0.88942500000000002</v>
+      </c>
+      <c r="J3" s="123">
+        <v>7991</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="125" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="125"/>
+      <c r="G4" s="124">
+        <v>0.74582199999999998</v>
+      </c>
+      <c r="H4" s="124">
+        <v>0.87918200000000002</v>
+      </c>
+      <c r="I4" s="124">
+        <v>0.80703000000000003</v>
+      </c>
+      <c r="J4" s="123">
+        <v>2690</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="125" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="124">
+        <v>0.85136100000000003</v>
+      </c>
+      <c r="C5" s="124">
+        <v>0.83676600000000001</v>
+      </c>
+      <c r="D5" s="124">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="E5" s="123">
+        <v>30392</v>
+      </c>
+      <c r="F5" s="124"/>
+      <c r="G5" s="124">
+        <v>0.97500500000000001</v>
+      </c>
+      <c r="H5" s="124">
+        <v>0.94929399999999997</v>
+      </c>
+      <c r="I5" s="124">
+        <v>0.961978</v>
+      </c>
+      <c r="J5" s="123">
+        <v>84606</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="125" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="124">
+        <v>0.83107699999999995</v>
+      </c>
+      <c r="C6" s="124">
+        <v>0.67498499999999995</v>
+      </c>
+      <c r="D6" s="124">
+        <v>0.74494199999999999</v>
+      </c>
+      <c r="E6" s="123">
+        <v>28011</v>
+      </c>
+      <c r="F6" s="124"/>
+      <c r="G6" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6" s="125" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="125" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="124">
+        <v>0.48210399999999998</v>
+      </c>
+      <c r="C7" s="124">
+        <v>0.74885500000000005</v>
+      </c>
+      <c r="D7" s="124">
+        <v>0.58657700000000002</v>
+      </c>
+      <c r="E7" s="123">
+        <v>10918</v>
+      </c>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124">
+        <v>0</v>
+      </c>
+      <c r="H7" s="124">
+        <v>0</v>
+      </c>
+      <c r="I7" s="124">
+        <v>0</v>
+      </c>
+      <c r="J7" s="123">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="125" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="124">
+        <v>0.13172600000000001</v>
+      </c>
+      <c r="C8" s="124">
+        <v>0.26960400000000001</v>
+      </c>
+      <c r="D8" s="124">
+        <v>0.176981</v>
+      </c>
+      <c r="E8" s="123">
+        <v>1135</v>
+      </c>
+      <c r="F8" s="124"/>
+      <c r="G8" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="125" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="125"/>
+      <c r="G9" s="124">
+        <v>0.234043</v>
+      </c>
+      <c r="H9" s="124">
+        <v>0.282051</v>
+      </c>
+      <c r="I9" s="124">
+        <v>0.25581399999999999</v>
+      </c>
+      <c r="J9" s="123">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="125" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="124">
+        <v>0.271565</v>
+      </c>
+      <c r="C10" s="124">
+        <v>0.12686600000000001</v>
+      </c>
+      <c r="D10" s="124">
+        <v>0.17294000000000001</v>
+      </c>
+      <c r="E10" s="123">
+        <v>670</v>
+      </c>
+      <c r="F10" s="124"/>
+      <c r="G10" s="124">
+        <v>0.71491099999999996</v>
+      </c>
+      <c r="H10" s="124">
+        <v>0.72175199999999995</v>
+      </c>
+      <c r="I10" s="124">
+        <v>0.71831500000000004</v>
+      </c>
+      <c r="J10" s="123">
+        <v>2717</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="125" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="124">
+        <v>0.37950099999999998</v>
+      </c>
+      <c r="C11" s="124">
+        <v>0.157471</v>
+      </c>
+      <c r="D11" s="124">
+        <v>0.222583</v>
+      </c>
+      <c r="E11" s="123">
+        <v>870</v>
+      </c>
+      <c r="F11" s="124"/>
+      <c r="G11" s="124">
+        <v>0.68630199999999997</v>
+      </c>
+      <c r="H11" s="124">
+        <v>0.71706400000000003</v>
+      </c>
+      <c r="I11" s="124">
+        <v>0.70134600000000002</v>
+      </c>
+      <c r="J11" s="123">
+        <v>10285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="120" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="121">
+        <v>0.28571400000000002</v>
+      </c>
+      <c r="C12" s="121">
+        <v>3.4009999999999999E-3</v>
+      </c>
+      <c r="D12" s="121">
+        <v>6.7229999999999998E-3</v>
+      </c>
+      <c r="E12" s="122">
+        <v>588</v>
+      </c>
+      <c r="F12" s="121"/>
+      <c r="G12" s="120" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="120" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="120" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" s="120" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="119" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="117">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="C13" s="117"/>
+      <c r="D13" s="118"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="117">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="H13" s="117"/>
+      <c r="I13" s="116"/>
+      <c r="J13" s="116"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="115"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="115"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="115"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="115"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="115"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="115"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="G13:H13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>